<commit_message>
Update generation research with Gen Z spending adjustments and new discretionary spending files
- Update Gen Z annual spend from $940 to $3,450 based on total online spending
- Add discretionary spending analysis files for all generations (2023-2030)
- Update market sizing calculations with revised Gen Z figures
- Modify data sources to reflect Piper Sandler/NIQ/DataReportal for Gen Z

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/generation-research/agentic_commerce_market_sizing_2025_2030.xlsx
+++ b/generation-research/agentic_commerce_market_sizing_2025_2030.xlsx
@@ -638,7 +638,7 @@
         <v>2025</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>153.6</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>0</v>
@@ -649,10 +649,10 @@
         <v>2026</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>280.1</v>
+        <v>292.5</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>82.40000000000001</v>
+        <v>82.8</v>
       </c>
     </row>
     <row r="4">
@@ -660,10 +660,10 @@
         <v>2027</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>449.4</v>
+        <v>468.8</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>60.4</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="5">
@@ -671,10 +671,10 @@
         <v>2028</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>638.4</v>
+        <v>663.8</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>42</v>
+        <v>41.6</v>
       </c>
     </row>
     <row r="6">
@@ -682,10 +682,10 @@
         <v>2029</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>808.3</v>
+        <v>837.2</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>26.6</v>
+        <v>26.1</v>
       </c>
     </row>
     <row r="7">
@@ -693,10 +693,10 @@
         <v>2030</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>933.8</v>
+        <v>964.5</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>15.5</v>
+        <v>15.2</v>
       </c>
     </row>
   </sheetData>
@@ -929,15 +929,15 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$940</t>
+          <t>$3,450</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2.381</v>
+        <v>8.737</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>67.0M × 21% × 18% × $940</t>
+          <t>67.0M × 21% × 18% × $3,450</t>
         </is>
       </c>
     </row>
@@ -1145,15 +1145,15 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>$940</t>
+          <t>$3,450</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>4.629</v>
+        <v>16.99</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>67.0M × 21% × 35% × $940</t>
+          <t>67.0M × 21% × 35% × $3,450</t>
         </is>
       </c>
     </row>
@@ -1361,15 +1361,15 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$940</t>
+          <t>$3,450</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>7.274</v>
+        <v>26.698</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>67.0M × 21% × 55% × $940</t>
+          <t>67.0M × 21% × 55% × $3,450</t>
         </is>
       </c>
     </row>
@@ -1577,15 +1577,15 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>$940</t>
+          <t>$3,450</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>9.523</v>
+        <v>34.95</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>67.0M × 21% × 72% × $940</t>
+          <t>67.0M × 21% × 72% × $3,450</t>
         </is>
       </c>
     </row>
@@ -1793,15 +1793,15 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>$940</t>
+          <t>$3,450</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>10.845</v>
+        <v>39.804</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>67.0M × 21% × 82% × $940</t>
+          <t>67.0M × 21% × 82% × $3,450</t>
         </is>
       </c>
     </row>
@@ -2009,15 +2009,15 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>$940</t>
+          <t>$3,450</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>11.506</v>
+        <v>42.231</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>67.0M × 21% × 87% × $940</t>
+          <t>67.0M × 21% × 87% × $3,450</t>
         </is>
       </c>
     </row>
@@ -2220,22 +2220,22 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>2.38</v>
+        <v>8.74</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>4.63</v>
+        <v>16.99</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>7.27</v>
+        <v>26.7</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>9.52</v>
+        <v>34.95</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>10.85</v>
+        <v>39.8</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>11.51</v>
+        <v>42.23</v>
       </c>
     </row>
     <row r="7">
@@ -2270,22 +2270,22 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>153.6</v>
+        <v>160</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>280.1</v>
+        <v>292.5</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>449.4</v>
+        <v>468.8</v>
       </c>
       <c r="E8" s="7" t="n">
-        <v>638.4</v>
+        <v>663.8</v>
       </c>
       <c r="F8" s="7" t="n">
-        <v>808.3</v>
+        <v>837.2</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>933.8</v>
+        <v>964.5</v>
       </c>
     </row>
   </sheetData>
@@ -2767,17 +2767,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$940</t>
+          <t>$3,450</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Bango Subscription Study</t>
+          <t>Piper Sandler/NIQ/DataReportal</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.thewrap.com/gen-z-most-subscribed-generation-study-bango/</t>
+          <t>https://www.pipersandler.com/teens</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
       </c>
       <c r="B7" s="8" t="inlineStr">
         <is>
-          <t>$940 based on subscription spending only</t>
+          <t>$3,450 based on total online spending (80% of shopping)</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
         <is>
-          <t>Conservative estimate; actual spending likely higher when including all categories</t>
+          <t>Calculated from Piper Sandler teen data, NIQ online shopping patterns, and DataReportal averages</t>
         </is>
       </c>
     </row>
@@ -3501,22 +3501,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gen Z Subscriptions</t>
+          <t>Gen Z Total Online Spending</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bango Study</t>
+          <t>Piper Sandler/NIQ/DataReportal</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.thewrap.com/gen-z-most-subscribed-generation-study-bango/</t>
+          <t>https://www.pipersandler.com/teens</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2024-2025</t>
         </is>
       </c>
     </row>

</xml_diff>